<commit_message>
Forgot to order table
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/example_lengths_sentiment_xlm-roberta.xlsx
+++ b/data_exploration/acl/tables/example_lengths_sentiment_xlm-roberta.xlsx
@@ -22,61 +22,61 @@
     <t>total</t>
   </si>
   <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Cantonese</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>Basque</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
     <t>Arabic</t>
   </si>
   <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
     <t>Algerian</t>
   </si>
   <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Greek</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>Basque</t>
-  </si>
-  <si>
-    <t>Finnish</t>
-  </si>
-  <si>
-    <t>Hebrew</t>
-  </si>
-  <si>
-    <t>Indonesian</t>
-  </si>
-  <si>
-    <t>Japanese</t>
-  </si>
-  <si>
-    <t>Korean</t>
-  </si>
-  <si>
     <t>Maltese</t>
-  </si>
-  <si>
-    <t>Norwegian</t>
-  </si>
-  <si>
-    <t>Slovak</t>
-  </si>
-  <si>
-    <t>Thai</t>
-  </si>
-  <si>
-    <t>Turkish</t>
-  </si>
-  <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>Cantonese</t>
   </si>
 </sst>
 </file>
@@ -465,19 +465,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>35841</v>
+        <v>4939</v>
       </c>
       <c r="C2">
-        <v>19755</v>
+        <v>4187</v>
       </c>
       <c r="D2">
-        <v>27713</v>
+        <v>4872</v>
       </c>
       <c r="E2">
-        <v>32492</v>
+        <v>4937</v>
       </c>
       <c r="F2">
-        <v>34807</v>
+        <v>4939</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -485,19 +485,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>564</v>
+        <v>1029</v>
       </c>
       <c r="C3">
-        <v>543</v>
+        <v>996</v>
       </c>
       <c r="D3">
-        <v>563</v>
+        <v>1027</v>
       </c>
       <c r="E3">
-        <v>564</v>
+        <v>1029</v>
       </c>
       <c r="F3">
-        <v>564</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -505,19 +505,19 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4939</v>
+        <v>3724</v>
       </c>
       <c r="C4">
-        <v>4187</v>
+        <v>3417</v>
       </c>
       <c r="D4">
-        <v>4872</v>
+        <v>3652</v>
       </c>
       <c r="E4">
-        <v>4937</v>
+        <v>3708</v>
       </c>
       <c r="F4">
-        <v>4939</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -525,19 +525,19 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>462</v>
+        <v>2675</v>
       </c>
       <c r="C5">
-        <v>458</v>
+        <v>2583</v>
       </c>
       <c r="D5">
-        <v>462</v>
+        <v>2674</v>
       </c>
       <c r="E5">
-        <v>462</v>
+        <v>2675</v>
       </c>
       <c r="F5">
-        <v>462</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -545,19 +545,19 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1029</v>
+        <v>462</v>
       </c>
       <c r="C6">
-        <v>996</v>
+        <v>458</v>
       </c>
       <c r="D6">
-        <v>1027</v>
+        <v>462</v>
       </c>
       <c r="E6">
-        <v>1029</v>
+        <v>462</v>
       </c>
       <c r="F6">
-        <v>1029</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -565,19 +565,19 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>789</v>
+        <v>19292</v>
       </c>
       <c r="C7">
-        <v>778</v>
+        <v>8987</v>
       </c>
       <c r="D7">
-        <v>788</v>
+        <v>13817</v>
       </c>
       <c r="E7">
-        <v>789</v>
+        <v>18268</v>
       </c>
       <c r="F7">
-        <v>789</v>
+        <v>19159</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -585,19 +585,19 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>1355</v>
+        <v>2384</v>
       </c>
       <c r="C8">
-        <v>823</v>
+        <v>2137</v>
       </c>
       <c r="D8">
-        <v>1140</v>
+        <v>2329</v>
       </c>
       <c r="E8">
-        <v>1297</v>
+        <v>2378</v>
       </c>
       <c r="F8">
-        <v>1344</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -605,19 +605,19 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>8702</v>
+        <v>8103</v>
       </c>
       <c r="C9">
-        <v>7307</v>
+        <v>7467</v>
       </c>
       <c r="D9">
-        <v>8239</v>
+        <v>8000</v>
       </c>
       <c r="E9">
-        <v>8581</v>
+        <v>8090</v>
       </c>
       <c r="F9">
-        <v>8663</v>
+        <v>8103</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -625,19 +625,19 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>100307</v>
+        <v>31217</v>
       </c>
       <c r="C10">
-        <v>97565</v>
+        <v>1122</v>
       </c>
       <c r="D10">
-        <v>100022</v>
+        <v>12852</v>
       </c>
       <c r="E10">
-        <v>100254</v>
+        <v>31217</v>
       </c>
       <c r="F10">
-        <v>100307</v>
+        <v>31217</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -645,19 +645,19 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>13976</v>
+        <v>100307</v>
       </c>
       <c r="C11">
-        <v>5394</v>
+        <v>97565</v>
       </c>
       <c r="D11">
-        <v>9677</v>
+        <v>100022</v>
       </c>
       <c r="E11">
-        <v>12511</v>
+        <v>100254</v>
       </c>
       <c r="F11">
-        <v>13710</v>
+        <v>100307</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -665,19 +665,19 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>3237</v>
+        <v>1355</v>
       </c>
       <c r="C12">
-        <v>2818</v>
+        <v>823</v>
       </c>
       <c r="D12">
-        <v>3227</v>
+        <v>1140</v>
       </c>
       <c r="E12">
-        <v>3237</v>
+        <v>1297</v>
       </c>
       <c r="F12">
-        <v>3237</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -685,19 +685,19 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>502</v>
+        <v>789</v>
       </c>
       <c r="C13">
-        <v>372</v>
+        <v>778</v>
       </c>
       <c r="D13">
-        <v>498</v>
+        <v>788</v>
       </c>
       <c r="E13">
-        <v>502</v>
+        <v>789</v>
       </c>
       <c r="F13">
-        <v>502</v>
+        <v>789</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -705,19 +705,19 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>2675</v>
+        <v>3237</v>
       </c>
       <c r="C14">
-        <v>2583</v>
+        <v>2818</v>
       </c>
       <c r="D14">
-        <v>2674</v>
+        <v>3227</v>
       </c>
       <c r="E14">
-        <v>2675</v>
+        <v>3237</v>
       </c>
       <c r="F14">
-        <v>2675</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -725,19 +725,19 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>3724</v>
+        <v>13976</v>
       </c>
       <c r="C15">
-        <v>3417</v>
+        <v>5394</v>
       </c>
       <c r="D15">
-        <v>3652</v>
+        <v>9677</v>
       </c>
       <c r="E15">
-        <v>3708</v>
+        <v>12511</v>
       </c>
       <c r="F15">
-        <v>3724</v>
+        <v>13710</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -745,19 +745,19 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>8103</v>
+        <v>915</v>
       </c>
       <c r="C16">
-        <v>7467</v>
+        <v>909</v>
       </c>
       <c r="D16">
-        <v>8000</v>
+        <v>915</v>
       </c>
       <c r="E16">
-        <v>8090</v>
+        <v>915</v>
       </c>
       <c r="F16">
-        <v>8103</v>
+        <v>915</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -765,19 +765,19 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>915</v>
+        <v>35841</v>
       </c>
       <c r="C17">
-        <v>909</v>
+        <v>19755</v>
       </c>
       <c r="D17">
-        <v>915</v>
+        <v>27713</v>
       </c>
       <c r="E17">
-        <v>915</v>
+        <v>32492</v>
       </c>
       <c r="F17">
-        <v>915</v>
+        <v>34807</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -785,19 +785,19 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>2384</v>
+        <v>8702</v>
       </c>
       <c r="C18">
-        <v>2137</v>
+        <v>7307</v>
       </c>
       <c r="D18">
-        <v>2329</v>
+        <v>8239</v>
       </c>
       <c r="E18">
-        <v>2378</v>
+        <v>8581</v>
       </c>
       <c r="F18">
-        <v>2384</v>
+        <v>8663</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -805,19 +805,19 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>19292</v>
+        <v>564</v>
       </c>
       <c r="C19">
-        <v>8987</v>
+        <v>543</v>
       </c>
       <c r="D19">
-        <v>13817</v>
+        <v>563</v>
       </c>
       <c r="E19">
-        <v>18268</v>
+        <v>564</v>
       </c>
       <c r="F19">
-        <v>19159</v>
+        <v>564</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -825,19 +825,19 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>31217</v>
+        <v>502</v>
       </c>
       <c r="C20">
-        <v>1122</v>
+        <v>372</v>
       </c>
       <c r="D20">
-        <v>12852</v>
+        <v>498</v>
       </c>
       <c r="E20">
-        <v>31217</v>
+        <v>502</v>
       </c>
       <c r="F20">
-        <v>31217</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>